<commit_message>
Updated Habitat Attribute (and related code) to not go reach by reach but by attribute
So now instead of running reach by reach, it runs for the entire attribute at once, code is much faster
</commit_message>
<xml_diff>
--- a/Output/Bull_Trout_Habitat_Quality_RESTORATOIN_Methow_Entiat_Wenatchee.xlsx
+++ b/Output/Bull_Trout_Habitat_Quality_RESTORATOIN_Methow_Entiat_Wenatchee.xlsx
@@ -568,12 +568,12 @@
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>Cover- Boulders,Off-Channel- Side-Channels</t>
+          <t>Cover-Wood,PoolQuantity&amp;Quality</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Coarse Substrate,Cover- Boulders,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,CoarseSubstrate,Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -661,12 +661,12 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>Cover- Boulders,Off-Channel- Side-Channels</t>
+          <t>Cover-Wood,PoolQuantity&amp;Quality</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>Cover- Boulders,Off-Channel- Side-Channels</t>
+          <t>Cover-Wood,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -754,7 +754,7 @@
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Cover- Boulders,Cover- Wood,Flow- Scour,Icing</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -842,7 +842,7 @@
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Cover- Wood,Flow- Scour,Icing</t>
+          <t>Stability,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -914,13 +914,13 @@
         <v>4</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T6">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U6">
-        <v>0.6222222222222222</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="V6">
         <v>5</v>
@@ -928,14 +928,9 @@
       <c r="W6">
         <v>1</v>
       </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Cover- Boulders,Cover- Wood,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1018,7 @@
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Cover- Wood,Flow- Scour,Icing</t>
+          <t>Stability,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -1111,12 +1106,12 @@
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>Cover- Boulders,Icing</t>
+          <t>Cover-Wood,Off-Channel-Side-Channels</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Cover- Boulders,Cover- Wood,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -1204,12 +1199,12 @@
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>Cover- Boulders</t>
+          <t>Cover-Wood,Riparian</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Coarse Substrate,Cover- Boulders,Cover- Wood,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,CoarseSubstrate,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -1297,29 +1292,29 @@
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Cover- Boulders,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Coarse Substrate,Cover- Boulders,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,CoarseSubstrate,Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mad River Lower 04</t>
+          <t>Nason Creek Lower 03</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Entiat</t>
+          <t>Wenatchee</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Lower Mad River</t>
+          <t>Lower Nason Creek</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1338,13 +1333,13 @@
         </is>
       </c>
       <c r="G11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H11">
         <v>5</v>
       </c>
       <c r="I11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J11">
         <v>5</v>
@@ -1353,34 +1348,34 @@
         <v>5</v>
       </c>
       <c r="L11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P11">
         <v>5</v>
       </c>
       <c r="Q11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T11">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U11">
-        <v>0.7777777777777778</v>
+        <v>0.8</v>
       </c>
       <c r="V11">
         <v>5</v>
@@ -1390,12 +1385,12 @@
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>Off-Channel- Side-Channels</t>
+          <t>Temperature-Rearing</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>Icing,Off-Channel- Side-Channels</t>
+          <t>Flow-SummerBaseFlow,Off-Channel-Floodplain,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -1483,12 +1478,12 @@
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>Off-Channel- Side-Channels</t>
+          <t>PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Cover- Boulders,Cover- Wood,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -1576,12 +1571,12 @@
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>Off-Channel- Side-Channels</t>
+          <t>PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Cover- Boulders,Cover- Wood,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -1669,12 +1664,12 @@
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>Off-Channel- Side-Channels</t>
+          <t>PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Cover- Boulders,Cover- Wood,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -1762,12 +1757,12 @@
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>Cover- Boulders,Flow- Scour,Icing</t>
+          <t>Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Cover- Boulders,Cover- Wood,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -1855,12 +1850,12 @@
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>Cover- Boulders,Flow- Scour,Icing</t>
+          <t>Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Cover- Boulders,Cover- Wood,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -1948,12 +1943,12 @@
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>Cover- Boulders</t>
+          <t>Cover-Wood,Riparian,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Coarse Substrate,Cover- Boulders,Cover- Wood,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,CoarseSubstrate,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -2041,12 +2036,12 @@
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>Cover- Boulders</t>
+          <t>Cover-Wood,Riparian,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Coarse Substrate,Cover- Boulders,Cover- Wood,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,CoarseSubstrate,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -2118,13 +2113,13 @@
         <v>1</v>
       </c>
       <c r="S19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T19">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="U19">
-        <v>0.5111111111111111</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="V19">
         <v>5</v>
@@ -2134,12 +2129,12 @@
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>Cover- Boulders</t>
+          <t>Cover-Wood,Riparian,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Coarse Substrate,Cover- Boulders,Cover- Wood,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,CoarseSubstrate,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
@@ -2208,13 +2203,13 @@
         <v>3</v>
       </c>
       <c r="S20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T20">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="U20">
-        <v>0.6444444444444445</v>
+        <v>0.6</v>
       </c>
       <c r="V20">
         <v>5</v>
@@ -2222,9 +2217,14 @@
       <c r="W20">
         <v>1</v>
       </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>Temperature-Rearing</t>
+        </is>
+      </c>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>% Fines/Embeddedness,Coarse Substrate,Cover- Boulders,Flow- Scour,Icing,Off-Channel- Side-Channels</t>
+          <t>Stability,CoarseSubstrate,Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to output for WebMap code and output
Made many updates to scripts to generate WebMap data tables
</commit_message>
<xml_diff>
--- a/Output/Bull_Trout_Habitat_Quality_RESTORATOIN_Methow_Entiat_Wenatchee.xlsx
+++ b/Output/Bull_Trout_Habitat_Quality_RESTORATOIN_Methow_Entiat_Wenatchee.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z19"/>
+  <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -492,7 +492,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Beaver Creek Lower 09</t>
+          <t>Beaver Creek North Fork 01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -521,49 +521,49 @@
         </is>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2">
+        <v>3</v>
+      </c>
+      <c r="R2">
+        <v>3</v>
+      </c>
+      <c r="S2">
         <v>2</v>
       </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>5</v>
-      </c>
-      <c r="M2">
-        <v>3</v>
-      </c>
-      <c r="N2">
-        <v>3</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>3</v>
-      </c>
-      <c r="Q2">
-        <v>3</v>
-      </c>
-      <c r="R2">
-        <v>3</v>
-      </c>
-      <c r="S2">
-        <v>3</v>
-      </c>
       <c r="T2">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="U2">
-        <v>0.5333333333333333</v>
+        <v>0.7111111111111111</v>
       </c>
       <c r="V2">
         <v>5</v>
@@ -578,29 +578,29 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>Stability,CoarseSubstrate,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian,Temperature-Rearing</t>
+          <t>Riparian,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>Stability,CoarseSubstrate,Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+          <t>Cover-Wood,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Beaver Creek North Fork 01</t>
+          <t>Entiat River Lake 01</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Upper Beaver Creek</t>
+          <t>Entiat River-Lake Creek</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -634,34 +634,34 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M3">
         <v>5</v>
       </c>
       <c r="N3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q3">
         <v>3</v>
       </c>
       <c r="R3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T3">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U3">
-        <v>0.7111111111111111</v>
+        <v>0.7555555555555555</v>
       </c>
       <c r="V3">
         <v>5</v>
@@ -671,24 +671,24 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>Cover-Wood,PoolQuantity&amp;Quality</t>
+          <t>Cover-Wood</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>Riparian,Temperature-Rearing</t>
+          <t>Flow-SummerBaseFlow,Off-Channel-Side-Channels,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>Cover-Wood,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+          <t>Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Side-Channels,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Entiat River Potato 07</t>
+          <t>Entiat River Lake 02</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -698,7 +698,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Entiat River-Potato Creek</t>
+          <t>Entiat River-Lake Creek</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -717,25 +717,25 @@
         </is>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>3</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J4">
         <v>5</v>
       </c>
       <c r="K4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <v>3</v>
       </c>
       <c r="M4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N4">
         <v>3</v>
@@ -744,22 +744,22 @@
         <v>5</v>
       </c>
       <c r="P4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q4">
         <v>5</v>
       </c>
       <c r="R4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S4">
         <v>3</v>
       </c>
       <c r="T4">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="U4">
-        <v>0.7111111111111111</v>
+        <v>0.5777777777777777</v>
       </c>
       <c r="V4">
         <v>5</v>
@@ -767,21 +767,26 @@
       <c r="W4">
         <v>1</v>
       </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>Cover-Wood,Off-Channel-Floodplain</t>
+        </is>
+      </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Temperature-Rearing</t>
+          <t>Stability,Flow-SummerBaseFlow,Off-Channel-Side-Channels,Riparian,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Temperature-Rearing</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Entiat River Potato 08</t>
+          <t>Entiat River Lake 04</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -791,7 +796,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Entiat River-Potato Creek</t>
+          <t>Entiat River-Lake Creek</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -810,49 +815,49 @@
         </is>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J5">
         <v>5</v>
       </c>
       <c r="K5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <v>3</v>
       </c>
       <c r="M5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N5">
         <v>3</v>
       </c>
       <c r="O5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S5">
         <v>3</v>
       </c>
       <c r="T5">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="U5">
-        <v>0.7333333333333333</v>
+        <v>0.6888888888888889</v>
       </c>
       <c r="V5">
         <v>5</v>
@@ -860,21 +865,26 @@
       <c r="W5">
         <v>1</v>
       </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>Cover-Wood,PoolQuantity&amp;Quality</t>
+        </is>
+      </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>Stability,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian,Temperature-Rearing</t>
+          <t>Flow-SummerBaseFlow,Off-Channel-Side-Channels,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>Stability,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian,Temperature-Rearing</t>
+          <t>Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Entiat River Preston 01</t>
+          <t>Entiat River Lake 08</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -884,7 +894,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Entiat River-Preston Creek</t>
+          <t>Entiat River-Lake Creek</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -903,25 +913,25 @@
         </is>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J6">
         <v>5</v>
       </c>
       <c r="K6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N6">
         <v>3</v>
@@ -930,22 +940,22 @@
         <v>3</v>
       </c>
       <c r="P6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q6">
         <v>5</v>
       </c>
       <c r="R6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T6">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="U6">
-        <v>0.6666666666666666</v>
+        <v>0.7555555555555555</v>
       </c>
       <c r="V6">
         <v>5</v>
@@ -953,21 +963,26 @@
       <c r="W6">
         <v>1</v>
       </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>Cover-Wood</t>
+        </is>
+      </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Temperature-Rearing</t>
+          <t>Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Temperature-Rearing</t>
+          <t>Cover-Wood,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Entiat River Preston 02</t>
+          <t>Entiat River Lake 09</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -977,7 +992,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Entiat River-Preston Creek</t>
+          <t>Entiat River-Lake Creek</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -996,49 +1011,49 @@
         </is>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J7">
         <v>5</v>
       </c>
       <c r="K7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N7">
         <v>3</v>
       </c>
       <c r="O7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T7">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="U7">
-        <v>0.7333333333333333</v>
+        <v>0.7555555555555555</v>
       </c>
       <c r="V7">
         <v>5</v>
@@ -1046,31 +1061,36 @@
       <c r="W7">
         <v>1</v>
       </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>Cover-Wood</t>
+        </is>
+      </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>Stability,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian,Temperature-Rearing</t>
+          <t>Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>Stability,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian,Temperature-Rearing</t>
+          <t>Cover-Wood,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Lake Creek Methow 01</t>
+          <t>Entiat River Lake 10</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Lake Creek (Methow)</t>
+          <t>Entiat River-Lake Creek</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1089,49 +1109,49 @@
         </is>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
+      <c r="P8">
+        <v>5</v>
+      </c>
+      <c r="Q8">
+        <v>5</v>
+      </c>
+      <c r="R8">
+        <v>5</v>
+      </c>
+      <c r="S8">
         <v>2</v>
       </c>
-      <c r="J8">
-        <v>5</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>3</v>
-      </c>
-      <c r="M8">
-        <v>3</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <v>3</v>
-      </c>
-      <c r="P8">
-        <v>3</v>
-      </c>
-      <c r="Q8">
-        <v>3</v>
-      </c>
-      <c r="R8">
-        <v>3</v>
-      </c>
-      <c r="S8">
-        <v>3</v>
-      </c>
       <c r="T8">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="U8">
-        <v>0.5333333333333333</v>
+        <v>0.7555555555555555</v>
       </c>
       <c r="V8">
         <v>5</v>
@@ -1141,39 +1161,39 @@
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>Cover-Wood,Off-Channel-Side-Channels</t>
+          <t>Cover-Wood</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>Stability,Flow-SummerBaseFlow,Off-Channel-Floodplain,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+          <t>Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+          <t>Cover-Wood,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Lake Creek Methow 02</t>
+          <t>Entiat River Potato 07</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Methow</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Lake Creek (Methow)</t>
+          <t>Entiat River-Potato Creek</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1190,16 +1210,16 @@
         <v>3</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L9">
         <v>3</v>
@@ -1211,25 +1231,25 @@
         <v>3</v>
       </c>
       <c r="O9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S9">
         <v>3</v>
       </c>
       <c r="T9">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="U9">
-        <v>0.4888888888888889</v>
+        <v>0.7111111111111111</v>
       </c>
       <c r="V9">
         <v>5</v>
@@ -1237,26 +1257,21 @@
       <c r="W9">
         <v>1</v>
       </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>Cover-Wood,Riparian</t>
-        </is>
-      </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>Stability,CoarseSubstrate,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Temperature-Rearing</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>Stability,CoarseSubstrate,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Mad River Lower 01</t>
+          <t>Entiat River Potato 08</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1266,7 +1281,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Lower Mad River</t>
+          <t>Entiat River-Potato Creek</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1285,49 +1300,49 @@
         </is>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P10">
         <v>3</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T10">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="U10">
-        <v>0.4444444444444444</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="V10">
         <v>5</v>
@@ -1335,36 +1350,31 @@
       <c r="W10">
         <v>1</v>
       </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>Stability,Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality</t>
-        </is>
-      </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>CoarseSubstrate,Riparian</t>
+          <t>Stability,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>Stability,CoarseSubstrate,Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian</t>
+          <t>Stability,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 05</t>
+          <t>Entiat River Preston 01</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Entiat River-Preston Creek</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1407,25 +1417,25 @@
         <v>3</v>
       </c>
       <c r="O11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P11">
         <v>3</v>
       </c>
       <c r="Q11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T11">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U11">
-        <v>0.5555555555555556</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="V11">
         <v>5</v>
@@ -1433,36 +1443,31 @@
       <c r="W11">
         <v>1</v>
       </c>
-      <c r="X11" t="inlineStr">
-        <is>
-          <t>PoolQuantity&amp;Quality,Temperature-Rearing</t>
-        </is>
-      </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 06</t>
+          <t>Entiat River Preston 02</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Entiat River-Preston Creek</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1493,7 +1498,7 @@
         <v>5</v>
       </c>
       <c r="K12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L12">
         <v>3</v>
@@ -1505,7 +1510,7 @@
         <v>3</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P12">
         <v>3</v>
@@ -1517,13 +1522,13 @@
         <v>3</v>
       </c>
       <c r="S12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T12">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="U12">
-        <v>0.5555555555555556</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="V12">
         <v>5</v>
@@ -1531,36 +1536,31 @@
       <c r="W12">
         <v>1</v>
       </c>
-      <c r="X12" t="inlineStr">
-        <is>
-          <t>PoolQuantity&amp;Quality,Temperature-Rearing</t>
-        </is>
-      </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian</t>
+          <t>Stability,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+          <t>Stability,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 07</t>
+          <t>Entiat River Preston 04</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Entiat River-Preston Creek</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1579,25 +1579,25 @@
         </is>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J13">
         <v>5</v>
       </c>
       <c r="K13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L13">
         <v>3</v>
       </c>
       <c r="M13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N13">
         <v>3</v>
@@ -1615,13 +1615,13 @@
         <v>3</v>
       </c>
       <c r="S13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T13">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="U13">
-        <v>0.5555555555555556</v>
+        <v>0.6444444444444445</v>
       </c>
       <c r="V13">
         <v>5</v>
@@ -1631,34 +1631,34 @@
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>PoolQuantity&amp;Quality,Temperature-Rearing</t>
+          <t>Cover-Wood,PoolQuantity&amp;Quality</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian</t>
+          <t>Flow-SummerBaseFlow,Off-Channel-Side-Channels,Riparian,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+          <t>Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 09</t>
+          <t>Entiat River Preston 05</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Entiat River-Lake Creek</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1677,13 +1677,13 @@
         </is>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J14">
         <v>5</v>
@@ -1695,31 +1695,31 @@
         <v>3</v>
       </c>
       <c r="M14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T14">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="U14">
-        <v>0.4222222222222222</v>
+        <v>0.7555555555555555</v>
       </c>
       <c r="V14">
         <v>5</v>
@@ -1729,34 +1729,34 @@
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,Temperature-Rearing</t>
+          <t>Cover-Wood</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>Stability,Flow-SummerBaseFlow,PoolQuantity&amp;Quality,Riparian</t>
+          <t>Flow-SummerBaseFlow,Off-Channel-Side-Channels,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+          <t>Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Side-Channels,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 10</t>
+          <t>Mad River Lower 01</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Wenatchee</t>
+          <t>Entiat</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Lower Nason Creek</t>
+          <t>Lower Mad River</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1778,19 +1778,19 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K15">
         <v>1</v>
       </c>
       <c r="L15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M15">
         <v>1</v>
@@ -1799,7 +1799,7 @@
         <v>1</v>
       </c>
       <c r="O15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P15">
         <v>3</v>
@@ -1811,13 +1811,13 @@
         <v>2</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="T15">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="U15">
-        <v>0.4222222222222222</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="V15">
         <v>5</v>
@@ -1827,24 +1827,24 @@
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,Temperature-Rearing</t>
+          <t>Stability,Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
         <is>
-          <t>Stability,Flow-SummerBaseFlow,PoolQuantity&amp;Quality,Riparian</t>
+          <t>CoarseSubstrate,Riparian</t>
         </is>
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+          <t>Stability,CoarseSubstrate,Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 12</t>
+          <t>Nason Creek Lower 05</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1882,10 +1882,10 @@
         <v>3</v>
       </c>
       <c r="J16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L16">
         <v>3</v>
@@ -1897,25 +1897,25 @@
         <v>3</v>
       </c>
       <c r="O16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S16">
         <v>1</v>
       </c>
       <c r="T16">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="U16">
-        <v>0.4666666666666667</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="V16">
         <v>5</v>
@@ -1925,24 +1925,24 @@
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>Cover-Wood,Riparian,Temperature-Rearing</t>
+          <t>PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>Stability,CoarseSubstrate,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian</t>
         </is>
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>Stability,CoarseSubstrate,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 13</t>
+          <t>Nason Creek Lower 06</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1980,10 +1980,10 @@
         <v>3</v>
       </c>
       <c r="J17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L17">
         <v>3</v>
@@ -1995,25 +1995,25 @@
         <v>3</v>
       </c>
       <c r="O17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S17">
         <v>1</v>
       </c>
       <c r="T17">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="U17">
-        <v>0.4666666666666667</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="V17">
         <v>5</v>
@@ -2023,24 +2023,24 @@
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>Cover-Wood,Riparian,Temperature-Rearing</t>
+          <t>PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>Stability,CoarseSubstrate,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian</t>
         </is>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>Stability,CoarseSubstrate,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Nason Creek Lower 14</t>
+          <t>Nason Creek Lower 07</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2078,10 +2078,10 @@
         <v>3</v>
       </c>
       <c r="J18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L18">
         <v>3</v>
@@ -2093,25 +2093,25 @@
         <v>3</v>
       </c>
       <c r="O18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S18">
         <v>1</v>
       </c>
       <c r="T18">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="U18">
-        <v>0.4666666666666667</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="V18">
         <v>5</v>
@@ -2121,110 +2121,600 @@
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>Cover-Wood,Riparian,Temperature-Rearing</t>
+          <t>PoolQuantity&amp;Quality,Temperature-Rearing</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>Stability,CoarseSubstrate,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,Riparian</t>
         </is>
       </c>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>Stability,CoarseSubstrate,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>Nason Creek Lower 09</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Wenatchee</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Lower Nason Creek</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>5</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>3</v>
+      </c>
+      <c r="P19">
+        <v>3</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>2</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>19</v>
+      </c>
+      <c r="U19">
+        <v>0.4222222222222222</v>
+      </c>
+      <c r="V19">
+        <v>5</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,Temperature-Rearing</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>Stability,Flow-SummerBaseFlow,PoolQuantity&amp;Quality,Riparian</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Nason Creek Lower 10</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Wenatchee</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Lower Nason Creek</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>3</v>
+      </c>
+      <c r="P20">
+        <v>3</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>2</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>19</v>
+      </c>
+      <c r="U20">
+        <v>0.4222222222222222</v>
+      </c>
+      <c r="V20">
+        <v>5</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,Temperature-Rearing</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>Stability,Flow-SummerBaseFlow,PoolQuantity&amp;Quality,Riparian</t>
+        </is>
+      </c>
+      <c r="Z20" t="inlineStr">
+        <is>
+          <t>Stability,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Nason Creek Lower 12</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Wenatchee</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Lower Nason Creek</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>3</v>
+      </c>
+      <c r="M21">
+        <v>3</v>
+      </c>
+      <c r="N21">
+        <v>3</v>
+      </c>
+      <c r="O21">
+        <v>3</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>21</v>
+      </c>
+      <c r="U21">
+        <v>0.4666666666666667</v>
+      </c>
+      <c r="V21">
+        <v>5</v>
+      </c>
+      <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>Cover-Wood,Riparian,Temperature-Rearing</t>
+        </is>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>Stability,CoarseSubstrate,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality</t>
+        </is>
+      </c>
+      <c r="Z21" t="inlineStr">
+        <is>
+          <t>Stability,CoarseSubstrate,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Nason Creek Lower 13</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Wenatchee</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Lower Nason Creek</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>3</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22">
+        <v>3</v>
+      </c>
+      <c r="O22">
+        <v>3</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>21</v>
+      </c>
+      <c r="U22">
+        <v>0.4666666666666667</v>
+      </c>
+      <c r="V22">
+        <v>5</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>Cover-Wood,Riparian,Temperature-Rearing</t>
+        </is>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>Stability,CoarseSubstrate,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality</t>
+        </is>
+      </c>
+      <c r="Z22" t="inlineStr">
+        <is>
+          <t>Stability,CoarseSubstrate,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Nason Creek Lower 14</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Wenatchee</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Lower Nason Creek</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23">
+        <v>3</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>3</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <v>3</v>
+      </c>
+      <c r="O23">
+        <v>3</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>21</v>
+      </c>
+      <c r="U23">
+        <v>0.4666666666666667</v>
+      </c>
+      <c r="V23">
+        <v>5</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>Cover-Wood,Riparian,Temperature-Rearing</t>
+        </is>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>Stability,CoarseSubstrate,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality</t>
+        </is>
+      </c>
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>Stability,CoarseSubstrate,Cover-Wood,Flow-SummerBaseFlow,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>Nason Creek Lower 15</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>Wenatchee</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>Lower Nason Creek</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="G19">
-        <v>3</v>
-      </c>
-      <c r="H19">
-        <v>3</v>
-      </c>
-      <c r="I19">
-        <v>3</v>
-      </c>
-      <c r="J19">
-        <v>3</v>
-      </c>
-      <c r="K19">
-        <v>3</v>
-      </c>
-      <c r="L19">
-        <v>5</v>
-      </c>
-      <c r="M19">
-        <v>3</v>
-      </c>
-      <c r="N19">
-        <v>3</v>
-      </c>
-      <c r="O19">
-        <v>3</v>
-      </c>
-      <c r="P19">
-        <v>3</v>
-      </c>
-      <c r="R19">
-        <v>3</v>
-      </c>
-      <c r="S19">
-        <v>1</v>
-      </c>
-      <c r="T19">
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <v>3</v>
+      </c>
+      <c r="L24">
+        <v>5</v>
+      </c>
+      <c r="M24">
+        <v>3</v>
+      </c>
+      <c r="N24">
+        <v>3</v>
+      </c>
+      <c r="O24">
+        <v>3</v>
+      </c>
+      <c r="P24">
+        <v>3</v>
+      </c>
+      <c r="R24">
+        <v>3</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
         <v>27</v>
       </c>
-      <c r="U19">
+      <c r="U24">
         <v>0.6</v>
       </c>
-      <c r="V19">
-        <v>5</v>
-      </c>
-      <c r="W19">
-        <v>1</v>
-      </c>
-      <c r="X19" t="inlineStr">
+      <c r="V24">
+        <v>5</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24" t="inlineStr">
         <is>
           <t>Temperature-Rearing</t>
         </is>
       </c>
-      <c r="Y19" t="inlineStr">
+      <c r="Y24" t="inlineStr">
         <is>
           <t>Stability,CoarseSubstrate,Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian</t>
         </is>
       </c>
-      <c r="Z19" t="inlineStr">
+      <c r="Z24" t="inlineStr">
         <is>
           <t>Stability,CoarseSubstrate,Cover-Wood,Off-Channel-Floodplain,Off-Channel-Side-Channels,PoolQuantity&amp;Quality,Riparian,Temperature-Rearing</t>
         </is>

</xml_diff>